<commit_message>
Add new loose game
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\slotmachine\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19125" windowHeight="10665" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19125" windowHeight="10665" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="basic" sheetId="1" r:id="rId1"/>
     <sheet name="wild cherry" sheetId="2" r:id="rId2"/>
     <sheet name="progressive" sheetId="3" r:id="rId3"/>
+    <sheet name="loose" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
   <si>
     <t>Slot 1</t>
   </si>
@@ -137,12 +138,39 @@
   </si>
   <si>
     <t>Plus every spin adds 0.05 coins to progressive</t>
+  </si>
+  <si>
+    <t>Heart</t>
+  </si>
+  <si>
+    <t>Gold Bar</t>
+  </si>
+  <si>
+    <t>Horseshoe</t>
+  </si>
+  <si>
+    <t>Heart+Any+Any</t>
+  </si>
+  <si>
+    <t>Heart+Heart+Any</t>
+  </si>
+  <si>
+    <t>Gold Bar+Any+Any</t>
+  </si>
+  <si>
+    <t>Gold Bar+Gold Bar+Any</t>
+  </si>
+  <si>
+    <t>Gold Bar+Gold Bar+Gold Bar</t>
+  </si>
+  <si>
+    <t>Horseshoe+Horseshoe+Horseshoe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -1076,7 +1104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -1373,4 +1401,304 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B2:B7)*SUM(C2:C7)*SUM(D2:D7)</f>
+        <v>41760</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11">
+        <f>B2*SUM(C3:C7)*SUM(D2:D7)</f>
+        <v>5625</v>
+      </c>
+      <c r="C11" s="2">
+        <f>B11/$B$8</f>
+        <v>0.13469827586206898</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <f>C11*D11</f>
+        <v>0.26939655172413796</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12">
+        <f>B2*C2*SUM(D2:D7)</f>
+        <v>900</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" ref="C12:C16" si="0">B12/$B$8</f>
+        <v>2.1551724137931036E-2</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" ref="E12:E16" si="1">C12*D12</f>
+        <v>8.6206896551724144E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13">
+        <f>B3*C3*D3</f>
+        <v>864</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>2.0689655172413793E-2</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.10344827586206896</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14">
+        <f>B4*C4*D4</f>
+        <v>320</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>7.6628352490421452E-3</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5977011494252873E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <f>B5*C5*D5</f>
+        <v>180</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>4.3103448275862068E-3</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>4.3103448275862072E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16">
+        <f>B6*SUM(C2:C5)*SUM(D2:D6)</f>
+        <v>1170</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>2.8017241379310345E-2</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.28017241379310343</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17">
+        <f>B6*C6*SUM(D2:D5)</f>
+        <v>129</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" ref="C17:C18" si="2">B17/$B$8</f>
+        <v>3.0890804597701149E-3</v>
+      </c>
+      <c r="D17">
+        <v>25</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" ref="E17:E18" si="3">C17*D17</f>
+        <v>7.7227011494252873E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18">
+        <f>B6*C6*D6</f>
+        <v>6</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="2"/>
+        <v>1.4367816091954023E-4</v>
+      </c>
+      <c r="D18">
+        <v>1000</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="3"/>
+        <v>0.14367816091954022</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1">
+        <f>SUM(C11:C19)</f>
+        <v>0.22016283524904215</v>
+      </c>
+      <c r="E20" s="1">
+        <f>SUM(E11:E19)</f>
+        <v>1.0492097701149423</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add everyone wins tournament machine
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\slotmachine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\slotmachine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B622F8D8-DF29-4B4C-B0E3-91C4C80A3A7D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19125" windowHeight="10665" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19125" windowHeight="10665" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="basic" sheetId="1" r:id="rId1"/>
@@ -20,6 +19,7 @@
     <sheet name="tournament" sheetId="6" r:id="rId5"/>
     <sheet name="tournament2" sheetId="7" r:id="rId6"/>
     <sheet name="tournament3" sheetId="8" r:id="rId7"/>
+    <sheet name="tournament4" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="64">
   <si>
     <t>Slot 1</t>
   </si>
@@ -211,12 +211,24 @@
   </si>
   <si>
     <t>Steak+Steak+Any</t>
+  </si>
+  <si>
+    <t>Heart+Heart+Heart</t>
+  </si>
+  <si>
+    <t>Orange+Any+Any</t>
+  </si>
+  <si>
+    <t>Seven+Any+Any</t>
+  </si>
+  <si>
+    <t>Seven+Seven+Any</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -567,7 +579,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -867,7 +879,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1147,7 +1159,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1450,7 +1462,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1750,7 +1762,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2024,7 +2036,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2304,10 +2316,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8691DFE2-482E-47AD-BB1E-BBBB7B9DDB75}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2601,4 +2613,370 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B2:B7)*SUM(C2:C7)*SUM(D2:D7)</f>
+        <v>12312</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f>B2*SUM(C2:C6)*SUM(D2:D6)-B12</f>
+        <v>3408</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" ref="C11:C21" si="0">B11/$B$8</f>
+        <v>0.27680311890838205</v>
+      </c>
+      <c r="D11">
+        <v>0.2</v>
+      </c>
+      <c r="E11" s="1">
+        <f>C11*D11</f>
+        <v>5.5360623781676416E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12">
+        <f>B2*C2*D2</f>
+        <v>480</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>3.8986354775828458E-2</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" ref="E12:E21" si="1">C12*D12</f>
+        <v>0.15594541910331383</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <f>B3*SUM(C2:C6)*SUM(D2:D6)-B14</f>
+        <v>2496</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.20272904483430798</v>
+      </c>
+      <c r="D13">
+        <v>0.2</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>4.05458089668616E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14">
+        <f>B3*C3*D3</f>
+        <v>96</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>7.7972709551656916E-3</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="1"/>
+        <v>4.6783625730994149E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15">
+        <f>B4*SUM(C2:C6)*SUM(D2:D6)-B16</f>
+        <v>2492</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.20240415854450941</v>
+      </c>
+      <c r="D15">
+        <v>0.2</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0480831708901883E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <f>B4*C4*D4</f>
+        <v>100</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>8.1221572449642621E-3</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>6.4977257959714096E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17">
+        <f>B5*SUM(C2:C6)*SUM(D2:D6)-B18</f>
+        <v>2544</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.20662768031189083</v>
+      </c>
+      <c r="D17">
+        <v>0.2</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="1"/>
+        <v>4.1325536062378168E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18">
+        <f>B5*C5*D5</f>
+        <v>48</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>3.8986354775828458E-3</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="1"/>
+        <v>3.8986354775828458E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19">
+        <f>B6*SUM(C2:C5)*SUM(D2:D6)</f>
+        <v>600</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>4.8732943469785572E-2</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="1"/>
+        <v>0.48732943469785572</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20">
+        <f>B6*C6*SUM(D2:D5)</f>
+        <v>40</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>3.2488628979857048E-3</v>
+      </c>
+      <c r="D20">
+        <v>20</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="1"/>
+        <v>6.4977257959714096E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <f>B6*C6*D6</f>
+        <v>8</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>6.4977257959714096E-4</v>
+      </c>
+      <c r="D21">
+        <v>50</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="1"/>
+        <v>3.2488628979857048E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="1">
+        <f>SUM(C11:C22)</f>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="E23" s="1">
+        <f>SUM(E11:E22)</f>
+        <v>1.0692007797270953</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="1">
+        <f>SUMIF(D11:D21,"&gt;1",C11:C21)</f>
+        <v>0.11143599740090968</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add new tournament machine
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\slotmachine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gsdri\Code\slotmachine\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CD4B39-A72B-40D5-9DF4-C816F7DF52CE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19125" windowHeight="10665" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19130" windowHeight="10670" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="basic" sheetId="1" r:id="rId1"/>
@@ -20,8 +21,9 @@
     <sheet name="tournament2" sheetId="7" r:id="rId6"/>
     <sheet name="tournament3" sheetId="8" r:id="rId7"/>
     <sheet name="tournament4" sheetId="9" r:id="rId8"/>
+    <sheet name="tournament5" sheetId="10" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="77">
   <si>
     <t>Slot 1</t>
   </si>
@@ -223,12 +225,51 @@
   </si>
   <si>
     <t>Seven+Seven+Any</t>
+  </si>
+  <si>
+    <t>Maggie</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>Marge</t>
+  </si>
+  <si>
+    <t>Bart</t>
+  </si>
+  <si>
+    <t>Homer</t>
+  </si>
+  <si>
+    <t>Maggie+Any+Any</t>
+  </si>
+  <si>
+    <t>Maggie+Maggie+Any</t>
+  </si>
+  <si>
+    <t>Lisa+Lisa+Lisa</t>
+  </si>
+  <si>
+    <t>Marge+Marge+Marge</t>
+  </si>
+  <si>
+    <t>Bart+Bart+Bart</t>
+  </si>
+  <si>
+    <t>Homer+Homer+Homer</t>
+  </si>
+  <si>
+    <t>Homer+Homer+Any</t>
+  </si>
+  <si>
+    <t>Homer+Any+Any</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -579,21 +620,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -618,7 +659,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -632,7 +673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -646,7 +687,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -660,7 +701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -674,7 +715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -683,7 +724,7 @@
         <v>38012</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -697,7 +738,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -717,7 +758,7 @@
         <v>0.29864253393665158</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -737,7 +778,7 @@
         <v>0.10859728506787331</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -757,7 +798,7 @@
         <v>0.13469430706092814</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -777,7 +818,7 @@
         <v>5.0510365147848055E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -797,7 +838,7 @@
         <v>4.7353467326107547E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -817,7 +858,7 @@
         <v>0.24886877828054296</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -837,7 +878,7 @@
         <v>8.8393139008734078E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -857,10 +898,10 @@
         <v>2.1045985478270017E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -879,21 +920,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -904,7 +945,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -918,7 +959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -932,7 +973,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -946,7 +987,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -960,7 +1001,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -974,7 +1015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -983,7 +1024,7 @@
         <v>34476</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -997,7 +1038,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1017,7 +1058,7 @@
         <v>0.32109293421510615</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1037,7 +1078,7 @@
         <v>3.4806822137138878E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1057,7 +1098,7 @@
         <v>0.14937927833855436</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1077,7 +1118,7 @@
         <v>0.23755656108597284</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1097,7 +1138,7 @@
         <v>8.1215918319990713E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1117,7 +1158,7 @@
         <v>7.8315349808562473E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1137,10 +1178,10 @@
         <v>8.7017055342847205E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1159,21 +1200,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.7265625" customWidth="1"/>
+    <col min="2" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1184,7 +1225,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1198,7 +1239,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1212,7 +1253,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1226,7 +1267,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1240,7 +1281,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1254,7 +1295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1263,7 +1304,7 @@
         <v>33456</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -1277,7 +1318,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1297,7 +1338,7 @@
         <v>0.29411764705882354</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1317,7 +1358,7 @@
         <v>0.11764705882352941</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1337,7 +1378,7 @@
         <v>9.5648015303682457E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1357,7 +1398,7 @@
         <v>5.7388809182209469E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1377,7 +1418,7 @@
         <v>5.3802008608321378E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1397,7 +1438,7 @@
         <v>0.26960784313725494</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1417,7 +1458,7 @@
         <v>4.7824007651841229E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1440,10 +1481,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1462,21 +1503,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1487,7 +1528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1501,7 +1542,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1515,7 +1556,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1529,7 +1570,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1543,7 +1584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1557,7 +1598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1566,7 +1607,7 @@
         <v>41760</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -1580,7 +1621,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1600,7 +1641,7 @@
         <v>0.26939655172413796</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1620,7 +1661,7 @@
         <v>8.6206896551724144E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1640,7 +1681,7 @@
         <v>0.10344827586206896</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1660,7 +1701,7 @@
         <v>4.5977011494252873E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1680,7 +1721,7 @@
         <v>4.3103448275862072E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1700,7 +1741,7 @@
         <v>0.28017241379310343</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1720,7 +1761,7 @@
         <v>7.7227011494252873E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1740,10 +1781,10 @@
         <v>0.14367816091954022</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1762,21 +1803,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1787,7 +1828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1801,7 +1842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1815,7 +1856,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1829,7 +1870,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1843,7 +1884,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1857,7 +1898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1871,7 +1912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1880,7 +1921,7 @@
         <v>39168</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>21</v>
       </c>
@@ -1894,7 +1935,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1914,7 +1955,7 @@
         <v>0.25939542483660133</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1934,7 +1975,7 @@
         <v>0.15956903594771241</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1954,7 +1995,7 @@
         <v>0.17667483660130717</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1974,7 +2015,7 @@
         <v>8.6805555555555552E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1994,7 +2035,7 @@
         <v>0.11233660130718953</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -2014,10 +2055,10 @@
         <v>0.25531045751633991</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -2036,21 +2077,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2061,7 +2102,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -2075,7 +2116,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -2089,7 +2130,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2103,7 +2144,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2117,7 +2158,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -2131,7 +2172,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2140,7 +2181,7 @@
         <v>22707</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -2154,7 +2195,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -2174,7 +2215,7 @@
         <v>0.32183908045977011</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -2194,7 +2235,7 @@
         <v>0.24521072796934865</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -2214,7 +2255,7 @@
         <v>0.13872374157748713</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2234,7 +2275,7 @@
         <v>7.3985995507993133E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2254,7 +2295,7 @@
         <v>0.16206456158893734</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2274,7 +2315,7 @@
         <v>0.10569427929713304</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -2294,10 +2335,10 @@
         <v>5.2847139648566521E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -2316,21 +2357,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2341,7 +2382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -2355,7 +2396,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -2369,7 +2410,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2383,7 +2424,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2397,7 +2438,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -2411,7 +2452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2420,7 +2461,7 @@
         <v>9450</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -2434,7 +2475,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -2454,7 +2495,7 @@
         <v>0.21714285714285714</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -2474,7 +2515,7 @@
         <v>0.13714285714285715</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -2494,7 +2535,7 @@
         <v>0.1219047619047619</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -2514,7 +2555,7 @@
         <v>7.6190476190476197E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -2534,7 +2575,7 @@
         <v>4.0634920634920635E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -2554,7 +2595,7 @@
         <v>0.32857142857142857</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -2574,7 +2615,7 @@
         <v>0.10582010582010581</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -2594,10 +2635,10 @@
         <v>4.2328042328042333E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2616,21 +2657,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2641,7 +2682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2655,7 +2696,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -2669,7 +2710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2683,7 +2724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -2697,7 +2738,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -2711,7 +2752,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2720,7 +2761,7 @@
         <v>12312</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -2734,7 +2775,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2754,7 +2795,7 @@
         <v>5.5360623781676416E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -2774,7 +2815,7 @@
         <v>0.15594541910331383</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -2794,7 +2835,7 @@
         <v>4.05458089668616E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -2814,7 +2855,7 @@
         <v>4.6783625730994149E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -2834,7 +2875,7 @@
         <v>4.0480831708901883E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -2854,7 +2895,7 @@
         <v>6.4977257959714096E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -2874,7 +2915,7 @@
         <v>4.1325536062378168E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -2894,7 +2935,7 @@
         <v>3.8986354775828458E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -2914,7 +2955,7 @@
         <v>0.48732943469785572</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -2934,7 +2975,7 @@
         <v>6.4977257959714096E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -2954,10 +2995,10 @@
         <v>3.2488628979857048E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -2970,10 +3011,310 @@
         <v>1.0692007797270953</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C24" s="1">
         <f>SUMIF(D11:D21,"&gt;1",C11:C21)</f>
         <v>0.11143599740090968</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFB6C747-826B-431D-925B-273DCC10B881}">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B2:B7)*SUM(C2:C7)*SUM(D2:D7)</f>
+        <v>36504</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11">
+        <f>B2*SUM(C3:C7)*SUM(D2:D7)</f>
+        <v>5148</v>
+      </c>
+      <c r="C11" s="2">
+        <f>B11/$B$8</f>
+        <v>0.14102564102564102</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <f>C11*D11</f>
+        <v>0.28205128205128205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12">
+        <f>B2*C2*SUM(D2:D7)</f>
+        <v>936</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" ref="C12:C18" si="0">B12/$B$8</f>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" ref="E12:E18" si="1">C12*D12</f>
+        <v>0.12820512820512819</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13">
+        <f>B3*C3*D3</f>
+        <v>288</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>7.889546351084813E-3</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>7.8895463510848127E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14">
+        <f>B4*C4*D4</f>
+        <v>288</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>7.889546351084813E-3</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="1"/>
+        <v>9.4674556213017763E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15">
+        <f>B5*C5*D5</f>
+        <v>144</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>3.9447731755424065E-3</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>5.9171597633136098E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16">
+        <f>B6*SUM(C2:C6)*SUM(D2:D6)-B17-B18</f>
+        <v>1716</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7008547008547008E-2</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.23504273504273504</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17">
+        <f>B6*C6*SUM(D2:D5)</f>
+        <v>304</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>8.3278544817006351E-3</v>
+      </c>
+      <c r="D17">
+        <v>25</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.20819636204251588</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18">
+        <f>B6*C6*D6</f>
+        <v>8</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>2.1915406530791147E-4</v>
+      </c>
+      <c r="D18">
+        <v>50</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0957703265395573E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1">
+        <f>SUM(C11:C19)</f>
+        <v>0.24194608809993429</v>
+      </c>
+      <c r="E20" s="1">
+        <f>SUM(E11:E19)</f>
+        <v>1.0971948279640586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>